<commit_message>
Partly upload of updated files/notebooks
</commit_message>
<xml_diff>
--- a/Stopword_results.xlsx
+++ b/Stopword_results.xlsx
@@ -37,10 +37,10 @@
     <t>Pred_SVM_747</t>
   </si>
   <si>
-    <t>Pred_SVM_imp</t>
+    <t>Pred_NB_imp</t>
   </si>
   <si>
-    <t>Pred_NB_imp</t>
+    <t>Pred_SVM_imp</t>
   </si>
 </sst>
 </file>
@@ -441,13 +441,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -610,13 +610,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -633,13 +633,13 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -665,13 +665,13 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -686,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -738,16 +738,16 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -942,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -953,13 +953,13 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1081,13 +1081,13 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1099,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1113,22 +1113,22 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1465,13 +1465,13 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1506,10 +1506,10 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H35">
         <v>3</v>
@@ -1518,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1599,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1614,7 +1614,7 @@
         <v>2</v>
       </c>
       <c r="J38">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1657,13 +1657,13 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1675,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1785,13 +1785,13 @@
         <v>2</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -1803,10 +1803,10 @@
         <v>2</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1899,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2283,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="I59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J59">
         <v>1</v>
@@ -2361,13 +2361,13 @@
         <v>4</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="I62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62">
         <v>1</v>
@@ -2731,10 +2731,10 @@
         <v>5</v>
       </c>
       <c r="I73">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J73">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2827,10 +2827,10 @@
         <v>5</v>
       </c>
       <c r="I76">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J76">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2905,28 +2905,28 @@
         <v>100</v>
       </c>
       <c r="C79">
-        <v>0.7792207792207793</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="D79">
-        <v>0.7792207792207793</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="E79">
-        <v>0.7792207792207793</v>
+        <v>0.7922077922077922</v>
       </c>
       <c r="F79">
+        <v>0.8181818181818182</v>
+      </c>
+      <c r="G79">
+        <v>0.8181818181818182</v>
+      </c>
+      <c r="H79">
         <v>0.8051948051948052</v>
       </c>
-      <c r="G79">
-        <v>0.8051948051948052</v>
-      </c>
-      <c r="H79">
-        <v>0.7792207792207793</v>
-      </c>
       <c r="I79">
-        <v>0.8441558441558441</v>
+        <v>0.7922077922077922</v>
       </c>
       <c r="J79">
-        <v>0.7792207792207793</v>
+        <v>0.8181818181818182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>